<commit_message>
a few more files for transportation in BC EMH project
</commit_message>
<xml_diff>
--- a/csv/policies/reference/Ref_LDV ZEV/formula_Ref_LDV ZEV_BC.xlsx
+++ b/csv/policies/reference/Ref_LDV ZEV/formula_Ref_LDV ZEV_BC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\xCIMS\cims-models\csv\policies\reference\Ref_LDV ZEV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{05747BAE-0E40-4343-B92C-4C0ED75AA16D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42CCDB72-F109-4024-960D-1570C27B8E41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B3591501-E185-4A3F-A3DB-0F2BD1858251}"/>
   </bookViews>
@@ -491,7 +491,7 @@
   <dimension ref="A1:X8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:X8"/>
+      <selection activeCell="T3" sqref="T3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -622,16 +622,16 @@
         <v>0.9</v>
       </c>
       <c r="T3">
-        <v>1</v>
+        <v>0.99</v>
       </c>
       <c r="U3">
-        <v>1</v>
+        <v>0.99</v>
       </c>
       <c r="V3">
-        <v>1</v>
+        <v>0.99</v>
       </c>
       <c r="W3">
-        <v>1</v>
+        <v>0.99</v>
       </c>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">

</xml_diff>